<commit_message>
aggiunto random (Da verificarne la correttezza)
</commit_message>
<xml_diff>
--- a/Grafici SRPT.xlsx
+++ b/Grafici SRPT.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alessio/Desktop/Università/Simulazione e Performance/Forest/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/filippo/Desktop/Network Simulation/Forest/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -27,10 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Lambda</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
   <si>
     <t>utilizzo</t>
   </si>
@@ -45,6 +42,12 @@
   </si>
   <si>
     <t>max q</t>
+  </si>
+  <si>
+    <t>SRPT</t>
+  </si>
+  <si>
+    <t>RANDOM (senza prelazione)</t>
   </si>
 </sst>
 </file>
@@ -308,11 +311,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1554236384"/>
-        <c:axId val="1400354800"/>
+        <c:axId val="-1430069200"/>
+        <c:axId val="-1430075056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1554236384"/>
+        <c:axId val="-1430069200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -415,12 +418,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1400354800"/>
+        <c:crossAx val="-1430075056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1400354800"/>
+        <c:axId val="-1430075056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120.0"/>
@@ -523,7 +526,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1554236384"/>
+        <c:crossAx val="-1430069200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -767,11 +770,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1524559520"/>
-        <c:axId val="1557510000"/>
+        <c:axId val="-1430045264"/>
+        <c:axId val="-1430041872"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1524559520"/>
+        <c:axId val="-1430045264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -875,7 +878,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1557510000"/>
+        <c:crossAx val="-1430041872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -883,7 +886,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1557510000"/>
+        <c:axId val="-1430041872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -995,7 +998,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1524559520"/>
+        <c:crossAx val="-1430045264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1364,7 +1367,6 @@
           <c:smooth val="1"/>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="r"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -1372,11 +1374,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1560120848"/>
-        <c:axId val="1573282928"/>
+        <c:axId val="-1444665248"/>
+        <c:axId val="-1444662048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1560120848"/>
+        <c:axId val="-1444665248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1465,12 +1467,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1573282928"/>
+        <c:crossAx val="-1444662048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1573282928"/>
+        <c:axId val="-1444662048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1572,7 +1574,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1560120848"/>
+        <c:crossAx val="-1444665248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1837,11 +1839,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1560182672"/>
-        <c:axId val="1574863264"/>
+        <c:axId val="-1429997088"/>
+        <c:axId val="-1429993328"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1560182672"/>
+        <c:axId val="-1429997088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1968,12 +1970,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1574863264"/>
+        <c:crossAx val="-1429993328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1574863264"/>
+        <c:axId val="-1429993328"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -2100,7 +2102,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1560182672"/>
+        <c:crossAx val="-1429997088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4303,16 +4305,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>522111</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>56445</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>239889</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>183445</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>101600</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>28223</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>651934</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4335,14 +4337,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>70555</xdr:rowOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>42332</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>522111</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>112889</xdr:rowOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>84666</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4363,16 +4365,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>479776</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>56445</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>634999</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>126999</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>522111</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>84668</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>677334</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>155222</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4394,15 +4396,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>169334</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:colOff>28223</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>42334</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>79</xdr:row>
-      <xdr:rowOff>197554</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>691445</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>112887</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4689,10 +4691,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:K8"/>
+  <dimension ref="C3:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4700,35 +4702,9 @@
     <col min="4" max="4" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2">
-        <v>3</v>
-      </c>
-      <c r="G2">
-        <v>4</v>
-      </c>
-      <c r="H2">
-        <v>5</v>
-      </c>
-      <c r="I2">
-        <v>6</v>
-      </c>
-      <c r="J2">
-        <v>7</v>
-      </c>
-      <c r="K2">
-        <v>8</v>
-      </c>
-    </row>
     <row r="3" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D3">
         <v>9.9999999999999995E-7</v>
@@ -4757,7 +4733,7 @@
     </row>
     <row r="4" spans="3:11" ht="17" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" s="1">
         <v>8.3377999999999994E-2</v>
@@ -4786,7 +4762,7 @@
     </row>
     <row r="5" spans="3:11" ht="17" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5">
         <v>8.2999999999999998E-5</v>
@@ -4815,7 +4791,7 @@
     </row>
     <row r="6" spans="3:11" ht="17" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D6" s="2">
         <v>831.48500000000001</v>
@@ -4844,7 +4820,7 @@
     </row>
     <row r="7" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D7">
         <v>3.6068999999999997E-2</v>
@@ -4873,7 +4849,7 @@
     </row>
     <row r="8" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -4898,6 +4874,60 @@
       </c>
       <c r="K8">
         <v>79272</v>
+      </c>
+    </row>
+    <row r="11" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="E11">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="F11">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="G11">
+        <v>8.0000000000000007E-5</v>
+      </c>
+      <c r="H11">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="I11">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="J11">
+        <v>2E-3</v>
+      </c>
+      <c r="K11">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aggiunto FIFO ai grafici
</commit_message>
<xml_diff>
--- a/Grafici SRPT.xlsx
+++ b/Grafici SRPT.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="8">
   <si>
     <t>utilizzo</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t>RANDOM (senza prelazione)</t>
+  </si>
+  <si>
+    <t>FIFO</t>
   </si>
 </sst>
 </file>
@@ -392,11 +395,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1386002928"/>
-        <c:axId val="-1386001360"/>
+        <c:axId val="539380560"/>
+        <c:axId val="539384672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1386002928"/>
+        <c:axId val="539380560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -508,12 +511,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1386001360"/>
+        <c:crossAx val="539384672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1386001360"/>
+        <c:axId val="539384672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120.0"/>
@@ -626,7 +629,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1386002928"/>
+        <c:crossAx val="539380560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -638,38 +641,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="t"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -989,11 +960,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1335383792"/>
-        <c:axId val="-1386731552"/>
+        <c:axId val="542331872"/>
+        <c:axId val="542334352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1335383792"/>
+        <c:axId val="542331872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1050,12 +1021,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1386731552"/>
+        <c:crossAx val="542334352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1386731552"/>
+        <c:axId val="542334352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1167,7 +1138,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1335383792"/>
+        <c:crossAx val="542331872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1179,38 +1150,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="t"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1283,12 +1222,19 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="it-IT"/>
-              <a:t>Respnse time e Waiting time medi all'aumentare di Lambda SRPT</a:t>
+              <a:t>Respnse time e Waiting time medi all'aumentare di Lambda (SRPT)</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.115993867748649"/>
+          <c:y val="0.0281249910033247"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1328,7 +1274,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Response Time SRPT</c:v>
+            <c:v>Response Time</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="22225" cap="rnd">
@@ -1357,10 +1303,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Foglio1!$D$3:$K$3</c:f>
+              <c:f>Foglio1!$D$3:$M$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1.0E-6</c:v>
                 </c:pt>
@@ -1384,16 +1330,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.004</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Foglio1!$D$6:$K$6</c:f>
+              <c:f>Foglio1!$D$6:$M$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0" formatCode="#,##0">
                   <c:v>831.485</c:v>
                 </c:pt>
@@ -1417,6 +1366,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>1284.439827</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>25276.67</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1427,7 +1379,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Waiting Time SRPT</c:v>
+            <c:v>Waiting Time</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="22225" cap="rnd">
@@ -1456,10 +1408,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Foglio1!$D$3:$K$3</c:f>
+              <c:f>Foglio1!$D$3:$M$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1.0E-6</c:v>
                 </c:pt>
@@ -1483,16 +1435,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.004</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Foglio1!$D$7:$K$7</c:f>
+              <c:f>Foglio1!$D$7:$M$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.036069</c:v>
                 </c:pt>
@@ -1516,6 +1471,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>703.20969</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>25212.67</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1530,12 +1488,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1386705808"/>
-        <c:axId val="-1386702048"/>
+        <c:axId val="542360048"/>
+        <c:axId val="542363808"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1386705808"/>
+        <c:axId val="542360048"/>
         <c:scaling>
+          <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1646,12 +1605,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1386702048"/>
+        <c:crossAx val="542363808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1386702048"/>
+        <c:axId val="542363808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1763,7 +1722,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1386705808"/>
+        <c:crossAx val="542360048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2118,6 +2077,105 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>FIFO</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Foglio1!$D$19:$K$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2E-6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0011</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Foglio1!$D$24:$K$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>56.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>50254.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>107356.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -2126,11 +2184,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1386680752"/>
-        <c:axId val="-1386676992"/>
+        <c:axId val="539420208"/>
+        <c:axId val="539423968"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1386680752"/>
+        <c:axId val="539420208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2243,12 +2301,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1386676992"/>
+        <c:crossAx val="539423968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1386676992"/>
+        <c:axId val="539423968"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -2362,7 +2420,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1386680752"/>
+        <c:crossAx val="539420208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2534,7 +2592,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Response Time RANDOM</c:v>
+            <c:v>Response Time</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="22225" cap="rnd">
@@ -2633,7 +2691,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Waiting Time Random</c:v>
+            <c:v>Waiting Time</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="22225" cap="rnd">
@@ -2736,11 +2794,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1355065808"/>
-        <c:axId val="-1302008336"/>
+        <c:axId val="539455488"/>
+        <c:axId val="539459984"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1355065808"/>
+        <c:axId val="539455488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2828,12 +2886,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1302008336"/>
+        <c:crossAx val="539459984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1302008336"/>
+        <c:axId val="539459984"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -2921,7 +2979,566 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1355065808"/>
+        <c:crossAx val="539455488"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="it-IT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="it-IT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="it-IT"/>
+              <a:t>response</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="it-IT" baseline="0"/>
+              <a:t> time e waitnig time all'aumentare di lambda (fifo)</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT" baseline="0"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Response Time</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Foglio1!$D$19:$K$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2E-6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0011</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Foglio1!$D$22:$K$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>834.844995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>832.2233335</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>836.44807</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>867.3715</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1190.6538</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6169.279101</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.244654974E7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.3436458E7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Waiting Time</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Foglio1!$D$19:$K$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.0E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2E-6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0011</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Foglio1!$D$23:$K$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.444995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.904935</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.3136</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>36.17794</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>356.9546</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5338.58663</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.2445716E7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.3435628E7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="r"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="573489456"/>
+        <c:axId val="573340064"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="573489456"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="it-IT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="573340064"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="573340064"/>
+        <c:scaling>
+          <c:logBase val="2.0"/>
+          <c:orientation val="minMax"/>
+          <c:max val="3.0777216E7"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="it-IT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="573489456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3202,6 +3819,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="241">
   <cs:axisTitle>
@@ -5802,20 +6459,540 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="241">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>804333</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>141112</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>819851</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>14112</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>141111</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>56444</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>507999</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>42334</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5836,16 +7013,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>508001</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>42333</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>14110</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>14111</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>395112</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>70555</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>395109</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5866,16 +7043,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>155222</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>112888</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>790223</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>155219</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>790223</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>42333</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>507999</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>155218</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5896,16 +7073,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>691443</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>183444</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>14110</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>28222</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>507999</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>141109</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>634999</xdr:colOff>
+      <xdr:row>122</xdr:row>
+      <xdr:rowOff>155223</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5928,16 +7105,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>522111</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>95955</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>197556</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>155222</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>324556</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>141111</xdr:rowOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>649111</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>155222</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5951,6 +7128,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>825501</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>152398</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>550333</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>155222</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Grafico 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6222,10 +7429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:K16"/>
+  <dimension ref="C3:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="B2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A48" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6235,7 +7442,7 @@
     <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
         <v>5</v>
       </c>
@@ -6263,8 +7470,11 @@
       <c r="K3">
         <v>4.0000000000000001E-3</v>
       </c>
+      <c r="L3">
+        <v>0.25</v>
+      </c>
     </row>
-    <row r="4" spans="3:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="3:13" ht="17" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
         <v>0</v>
       </c>
@@ -6292,8 +7502,11 @@
       <c r="K4">
         <v>99.998456000000004</v>
       </c>
+      <c r="L4">
+        <v>99.983975000000001</v>
+      </c>
     </row>
-    <row r="5" spans="3:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="3:13" ht="17" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
         <v>1</v>
       </c>
@@ -6321,8 +7534,11 @@
       <c r="K5">
         <v>0.99998399999999998</v>
       </c>
+      <c r="L5">
+        <v>0.99975000000000003</v>
+      </c>
     </row>
-    <row r="6" spans="3:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="3:13" ht="17" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
         <v>2</v>
       </c>
@@ -6350,8 +7566,12 @@
       <c r="K6" s="3">
         <v>1284.4398269999999</v>
       </c>
+      <c r="L6" s="3">
+        <v>25276.67</v>
+      </c>
+      <c r="M6" s="3"/>
     </row>
-    <row r="7" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
         <v>3</v>
       </c>
@@ -6379,8 +7599,12 @@
       <c r="K7">
         <v>703.20969000000002</v>
       </c>
+      <c r="L7" s="3">
+        <v>25212.67</v>
+      </c>
+      <c r="M7" s="3"/>
     </row>
-    <row r="8" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
         <v>4</v>
       </c>
@@ -6408,8 +7632,12 @@
       <c r="K8">
         <v>79272</v>
       </c>
+      <c r="L8" s="3">
+        <v>17669</v>
+      </c>
+      <c r="M8" s="3"/>
     </row>
-    <row r="11" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
         <v>6</v>
       </c>
@@ -6438,7 +7666,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="12" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
         <v>0</v>
       </c>
@@ -6467,7 +7695,7 @@
         <v>99.999835000000004</v>
       </c>
     </row>
-    <row r="13" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
         <v>1</v>
       </c>
@@ -6496,7 +7724,7 @@
         <v>0.99999979999999999</v>
       </c>
     </row>
-    <row r="14" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
         <v>2</v>
       </c>
@@ -6525,7 +7753,7 @@
         <v>7913445.71</v>
       </c>
     </row>
-    <row r="15" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
         <v>3</v>
       </c>
@@ -6554,7 +7782,7 @@
         <v>7912613.6740629999</v>
       </c>
     </row>
-    <row r="16" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C16" t="s">
         <v>4</v>
       </c>
@@ -6581,6 +7809,180 @@
       </c>
       <c r="K16" s="4">
         <v>107691</v>
+      </c>
+    </row>
+    <row r="19" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="E19">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="F19">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="G19">
+        <v>8.0000000000000007E-5</v>
+      </c>
+      <c r="H19">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="I19">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="J19">
+        <v>2E-3</v>
+      </c>
+      <c r="K19">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>8.3518999999999996E-2</v>
+      </c>
+      <c r="E20">
+        <v>0.16570199999999999</v>
+      </c>
+      <c r="F20">
+        <v>0.83318499999999995</v>
+      </c>
+      <c r="G20">
+        <v>6.6164699999999996</v>
+      </c>
+      <c r="H20">
+        <v>41.656100000000002</v>
+      </c>
+      <c r="I20">
+        <v>91.061199999999999</v>
+      </c>
+      <c r="J20">
+        <v>99.996870000000001</v>
+      </c>
+      <c r="K20">
+        <v>99.994125999999994</v>
+      </c>
+    </row>
+    <row r="21" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>8.3600000000000005E-4</v>
+      </c>
+      <c r="E21">
+        <v>1.6570000000000001E-3</v>
+      </c>
+      <c r="F21">
+        <v>8.3320000000000009E-3</v>
+      </c>
+      <c r="G21">
+        <v>6.6165000000000002E-2</v>
+      </c>
+      <c r="H21">
+        <v>0.41656199999999999</v>
+      </c>
+      <c r="I21">
+        <v>0.91061000000000003</v>
+      </c>
+      <c r="J21">
+        <v>0.99996700000000005</v>
+      </c>
+      <c r="K21">
+        <v>0.99994099999999997</v>
+      </c>
+    </row>
+    <row r="22" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <v>834.84499500000004</v>
+      </c>
+      <c r="E22">
+        <v>832.22333349999997</v>
+      </c>
+      <c r="F22" s="4">
+        <v>836.44807000000003</v>
+      </c>
+      <c r="G22" s="4">
+        <v>867.37149999999997</v>
+      </c>
+      <c r="H22" s="4">
+        <v>1190.6538</v>
+      </c>
+      <c r="I22" s="4">
+        <v>6169.2791010000001</v>
+      </c>
+      <c r="J22" s="4">
+        <v>12446549.74</v>
+      </c>
+      <c r="K22" s="4">
+        <v>13436458</v>
+      </c>
+    </row>
+    <row r="23" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23">
+        <v>0.44499499999999997</v>
+      </c>
+      <c r="E23">
+        <v>0.90493500000000004</v>
+      </c>
+      <c r="F23" s="4">
+        <v>4.3136000000000001</v>
+      </c>
+      <c r="G23" s="4">
+        <v>36.17794</v>
+      </c>
+      <c r="H23" s="4">
+        <v>356.95460000000003</v>
+      </c>
+      <c r="I23" s="4">
+        <v>5338.5866299999998</v>
+      </c>
+      <c r="J23" s="4">
+        <v>12445716</v>
+      </c>
+      <c r="K23" s="4">
+        <v>13435628</v>
+      </c>
+    </row>
+    <row r="24" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24" s="4">
+        <v>2</v>
+      </c>
+      <c r="G24" s="4">
+        <v>3</v>
+      </c>
+      <c r="H24" s="4">
+        <v>9</v>
+      </c>
+      <c r="I24" s="4">
+        <v>56</v>
+      </c>
+      <c r="J24" s="4">
+        <v>50254</v>
+      </c>
+      <c r="K24" s="4">
+        <v>107356</v>
       </c>
     </row>
   </sheetData>

</xml_diff>